<commit_message>
Plantilla para ejc de viabilidad
</commit_message>
<xml_diff>
--- a/LABORATORIO/PlantillaAlbertoGonzalez.xlsx
+++ b/LABORATORIO/PlantillaAlbertoGonzalez.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alberto\OneDrive\Documentos\GitHub\Gestion-de-Proyectos\LABORATORIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="6_{BAD6B766-0025-46F8-9DD1-079A69F0C6B5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="255" documentId="6_{BAD6B766-0025-46F8-9DD1-079A69F0C6B5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{F9939061-EE05-43A8-A935-5E6341316CB1}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3585" yWindow="1650" windowWidth="21600" windowHeight="11385" xr2:uid="{3EAC4CDE-D374-488D-8C8A-A6FF80133821}"/>
+    <workbookView xWindow="3225" yWindow="2190" windowWidth="21600" windowHeight="11385" xr2:uid="{3EAC4CDE-D374-488D-8C8A-A6FF80133821}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="66">
   <si>
     <t>INVERSIONES</t>
   </si>
@@ -160,6 +160,75 @@
   </si>
   <si>
     <t>GESTION DE TRÁFICO</t>
+  </si>
+  <si>
+    <t>PREVISION DE INGRESOS</t>
+  </si>
+  <si>
+    <t>SALUD ESTRUCTURAL Y CONTROL DE EDIFCIOS</t>
+  </si>
+  <si>
+    <t>GESTION DE TRAFICO</t>
+  </si>
+  <si>
+    <t>ESCENARIO 1 (1+4)</t>
+  </si>
+  <si>
+    <t>ESCENARIO 2 (2+3)</t>
+  </si>
+  <si>
+    <t>ESCENARIO 3 (1+2+3+4)</t>
+  </si>
+  <si>
+    <t>Gastos de personal</t>
+  </si>
+  <si>
+    <t>Alquileres</t>
+  </si>
+  <si>
+    <t>Gastos generales</t>
+  </si>
+  <si>
+    <t>Seguros y tributos</t>
+  </si>
+  <si>
+    <t>Aprovisionamientos</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>Amortizaciones</t>
+  </si>
+  <si>
+    <t>COSTES FIJOS (€)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AÑO 2 </t>
+  </si>
+  <si>
+    <t>INGRESOS TOTALES</t>
+  </si>
+  <si>
+    <t>COSTES FIJOS</t>
+  </si>
+  <si>
+    <t>AMORTIZACIONES</t>
+  </si>
+  <si>
+    <t>GASTOS VARIABLES</t>
+  </si>
+  <si>
+    <t>BENEFICIOS</t>
+  </si>
+  <si>
+    <t>IMPUESTOS</t>
+  </si>
+  <si>
+    <t>BENEFICIOS NETOS</t>
+  </si>
+  <si>
+    <t>BENEFICIOS ACUMULADOS</t>
   </si>
 </sst>
 </file>
@@ -183,7 +252,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,8 +283,92 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -238,11 +391,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -277,32 +487,184 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,7 +831,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -581,7 +943,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2700</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -590,7 +952,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -688,14 +1050,26 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>(Hoja1!$G$19,Hoja1!$H$19)</c:f>
+              <c:f>(Hoja1!$G$19,Hoja1!$H$19,Hoja1!$H$19,Hoja1!$I$19,Hoja1!$J$19,Hoja1!$K$19)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>43300</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1902,10 +2276,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3D7910-A5B9-4DC6-9781-64D99FA28BA6}">
-  <dimension ref="B3:K49"/>
+  <dimension ref="B3:K113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,28 +2329,32 @@
       <c r="K4" s="20"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="4"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="4">
+        <v>1500</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="4"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="4">
+        <v>2500</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -1992,7 +2370,7 @@
       <c r="F7" s="18"/>
       <c r="G7" s="5">
         <f>SUM(G5,G6)</f>
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="H7" s="5">
         <f>SUM(H5,H6)</f>
@@ -2012,16 +2390,16 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
@@ -2038,16 +2416,20 @@
       <c r="K9" s="20"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="4"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="4">
+        <v>2700</v>
+      </c>
       <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="I10" s="4">
+        <v>3600</v>
+      </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
@@ -2061,7 +2443,7 @@
       <c r="F11" s="18"/>
       <c r="G11" s="5">
         <f>SUM(G10)</f>
-        <v>0</v>
+        <v>2700</v>
       </c>
       <c r="H11" s="5">
         <f>SUM(H10)</f>
@@ -2069,7 +2451,7 @@
       </c>
       <c r="I11" s="5">
         <f>SUM(I10)</f>
-        <v>0</v>
+        <v>3600</v>
       </c>
       <c r="J11" s="5">
         <f>SUM(J10)</f>
@@ -2081,16 +2463,16 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="20" t="s">
@@ -2107,70 +2489,84 @@
       <c r="K13" s="20"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="4"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="4">
+        <v>3000</v>
+      </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="4"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="4">
+        <v>3600</v>
+      </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="4"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="4">
+        <v>3000</v>
+      </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="4"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="4">
+        <f>(6200+18500)</f>
+        <v>24700</v>
+      </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="J17" s="4">
+        <f>(5000+15000)</f>
+        <v>20000</v>
+      </c>
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="4"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="4">
+        <v>9000</v>
+      </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -2186,7 +2582,7 @@
       <c r="F19" s="18"/>
       <c r="G19" s="5">
         <f>SUM(G14:G18)</f>
-        <v>0</v>
+        <v>43300</v>
       </c>
       <c r="H19" s="5">
         <f>SUM(H14:H18)</f>
@@ -2198,7 +2594,7 @@
       </c>
       <c r="J19" s="5">
         <f>SUM(J14:J18)</f>
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="K19" s="5">
         <f>SUM(K14:K18)</f>
@@ -2206,16 +2602,16 @@
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
@@ -2227,7 +2623,7 @@
       <c r="F21" s="18"/>
       <c r="G21" s="3">
         <f>SUM(G7,G11,G19)</f>
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="H21" s="3">
         <f>SUM(H7,H11,H19)</f>
@@ -2235,11 +2631,11 @@
       </c>
       <c r="I21" s="3">
         <f>SUM(I7,I11,I19)</f>
-        <v>0</v>
+        <v>3600</v>
       </c>
       <c r="J21" s="3">
         <f>SUM(J7,J11,J19)</f>
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="K21" s="3">
         <f>SUM(K7,K11,K19)</f>
@@ -2247,13 +2643,13 @@
       </c>
     </row>
     <row r="28" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
       <c r="G28" s="7" t="s">
         <v>22</v>
       </c>
@@ -2267,18 +2663,22 @@
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="2:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="11">
+        <v>2500</v>
+      </c>
+      <c r="H29" s="11">
+        <v>10</v>
+      </c>
       <c r="I29" s="11">
         <f>PRODUCT(G29,H29)</f>
-        <v>0</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="30" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2289,331 +2689,1061 @@
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
+      <c r="G30" s="11">
+        <v>2500</v>
+      </c>
+      <c r="H30" s="11">
+        <v>8</v>
+      </c>
       <c r="I30" s="11">
         <f>PRODUCT(G30,H30)</f>
-        <v>0</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="31" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="11">
+        <v>2000</v>
+      </c>
+      <c r="H31" s="11">
+        <v>12</v>
+      </c>
       <c r="I31" s="11">
         <f>PRODUCT(G31,H31)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="13" t="s">
-        <v>25</v>
-      </c>
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="13"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11">
-        <f>PRODUCT(G32,H232)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="10" t="s">
+      <c r="G32" s="6"/>
+      <c r="H32" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="I33" s="4">
-        <f>SUM(I29,I30,I31,I32)</f>
-        <v>0</v>
+      <c r="I32" s="4">
+        <f>SUM(I29,I30,I31)</f>
+        <v>69000</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>24</v>
+      <c r="B34" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="11">
+        <v>500</v>
+      </c>
+      <c r="H34" s="11">
+        <v>20</v>
+      </c>
+      <c r="I34" s="11">
+        <f>PRODUCT(G34,H34)</f>
+        <v>10000</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C35" s="14"/>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
+      <c r="G35" s="11">
+        <v>750</v>
+      </c>
+      <c r="H35" s="11">
+        <v>10</v>
+      </c>
       <c r="I35" s="11">
         <f>PRODUCT(G35,H35)</f>
-        <v>0</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="14"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
+      <c r="G36" s="11">
+        <v>1000</v>
+      </c>
+      <c r="H36" s="11">
+        <v>8</v>
+      </c>
       <c r="I36" s="11">
         <f>PRODUCT(G36,H36)</f>
-        <v>0</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C37" s="14"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
+      <c r="G37" s="11">
+        <v>500</v>
+      </c>
+      <c r="H37" s="11">
+        <v>12</v>
+      </c>
       <c r="I37" s="11">
         <f>PRODUCT(G37,H37)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11">
-        <f>PRODUCT(G38,H38)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="10" t="s">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="I39" s="4">
-        <f>SUM(I35,I36,I37,I38)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B40" s="16" t="s">
+      <c r="I38" s="4">
+        <f>SUM(I34,I35,I36,I37)</f>
+        <v>31500</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="9" t="s">
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H40" s="9" t="s">
+      <c r="H39" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I40" s="8" t="s">
+      <c r="I39" s="8" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="11">
+        <v>1000</v>
+      </c>
+      <c r="H40" s="11">
+        <v>12</v>
+      </c>
+      <c r="I40" s="11">
+        <f>PRODUCT(G40,H40)</f>
+        <v>12000</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="14"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
+      <c r="G41" s="11">
+        <v>1500</v>
+      </c>
+      <c r="H41" s="11">
+        <v>8</v>
+      </c>
       <c r="I41" s="11">
         <f>PRODUCT(G41,H41)</f>
-        <v>0</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
+      <c r="G42" s="11">
+        <v>1000</v>
+      </c>
+      <c r="H42" s="11">
+        <v>20</v>
+      </c>
       <c r="I42" s="11">
         <f>PRODUCT(G42,H42)</f>
-        <v>0</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="14"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
+      <c r="G43" s="11">
+        <v>2000</v>
+      </c>
+      <c r="H43" s="11">
+        <v>10</v>
+      </c>
       <c r="I43" s="11">
         <f>PRODUCT(G43,H43)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11">
-        <f>PRODUCT(G44,H44)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="10" t="s">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="I45" s="4">
-        <f>SUM(I41,I42,I43,I44)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="I44" s="4">
+        <f>SUM(I40,I41,I42,I43)</f>
+        <v>64000</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B45" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
       <c r="F46" s="16"/>
-      <c r="G46" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H46" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I46" s="8" t="s">
-        <v>24</v>
+      <c r="G46" s="11">
+        <v>10000</v>
+      </c>
+      <c r="H46" s="11">
+        <v>4</v>
+      </c>
+      <c r="I46" s="11">
+        <f>PRODUCT(G46,H46)</f>
+        <v>40000</v>
       </c>
     </row>
     <row r="47" spans="2:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
+      <c r="B47" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="11">
+        <v>3000</v>
+      </c>
+      <c r="H47" s="11">
+        <v>4</v>
+      </c>
       <c r="I47" s="11">
         <f>PRODUCT(G47,H47)</f>
-        <v>0</v>
+        <v>12000</v>
       </c>
       <c r="J47" s="12"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11">
-        <f>PRODUCT(G48,H48)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="10" t="s">
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="I49" s="4">
-        <f>SUM(I47,I48)</f>
-        <v>0</v>
-      </c>
+      <c r="I48" s="4">
+        <f>SUM(I46,I47)</f>
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="22">
+        <f>SUM(I48,I44,I38,I32)</f>
+        <v>216500</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C53" s="27"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F53" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="G53" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H53" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="I53" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C54" s="34"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" s="34"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C56" s="34"/>
+      <c r="D56" s="35"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C57" s="34"/>
+      <c r="D57" s="35"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+    </row>
+    <row r="61" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" s="27"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F61" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="G61" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H61" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="I61" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C62" s="31"/>
+      <c r="D62" s="32"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C63" s="31"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C64" s="31"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B68" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C68" s="27"/>
+      <c r="D68" s="28"/>
+      <c r="E68" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F68" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="G68" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H68" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="I68" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B69" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C69" s="31"/>
+      <c r="D69" s="32"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B70" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C70" s="31"/>
+      <c r="D70" s="32"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" s="31"/>
+      <c r="D71" s="32"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B72" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C72" s="31"/>
+      <c r="D72" s="32"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B73" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C73" s="31"/>
+      <c r="D73" s="32"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B74" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C74" s="31"/>
+      <c r="D74" s="32"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B75" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C75" s="31"/>
+      <c r="D75" s="32"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B76" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C76" s="37"/>
+      <c r="D76" s="38"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B81" s="39"/>
+      <c r="C81" s="39"/>
+      <c r="D81" s="40"/>
+      <c r="E81" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F81" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="G81" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H81" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="I81" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B82" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="C82" s="42"/>
+      <c r="D82" s="42"/>
+      <c r="E82" s="42"/>
+      <c r="F82" s="42"/>
+      <c r="G82" s="42"/>
+      <c r="H82" s="42"/>
+      <c r="I82" s="43"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C83" s="45"/>
+      <c r="D83" s="46"/>
+      <c r="E83" s="47"/>
+      <c r="F83" s="47"/>
+      <c r="G83" s="47"/>
+      <c r="H83" s="47"/>
+      <c r="I83" s="47"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B84" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C84" s="45"/>
+      <c r="D84" s="46"/>
+      <c r="E84" s="47"/>
+      <c r="F84" s="47"/>
+      <c r="G84" s="47"/>
+      <c r="H84" s="47"/>
+      <c r="I84" s="47"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B85" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C85" s="45"/>
+      <c r="D85" s="46"/>
+      <c r="E85" s="47"/>
+      <c r="F85" s="47"/>
+      <c r="G85" s="47"/>
+      <c r="H85" s="47"/>
+      <c r="I85" s="47"/>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B86" s="23"/>
+      <c r="C86" s="24"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="24"/>
+      <c r="H86" s="24"/>
+      <c r="I86" s="25"/>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B87" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="C87" s="49"/>
+      <c r="D87" s="50"/>
+      <c r="E87" s="54"/>
+      <c r="F87" s="54"/>
+      <c r="G87" s="54"/>
+      <c r="H87" s="54"/>
+      <c r="I87" s="54"/>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B88" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="C88" s="49"/>
+      <c r="D88" s="50"/>
+      <c r="E88" s="54"/>
+      <c r="F88" s="54"/>
+      <c r="G88" s="54"/>
+      <c r="H88" s="54"/>
+      <c r="I88" s="54"/>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B89" s="23"/>
+      <c r="C89" s="24"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="24"/>
+      <c r="H89" s="24"/>
+      <c r="I89" s="25"/>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C90" s="49"/>
+      <c r="D90" s="49"/>
+      <c r="E90" s="49"/>
+      <c r="F90" s="49"/>
+      <c r="G90" s="49"/>
+      <c r="H90" s="49"/>
+      <c r="I90" s="50"/>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B91" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="C91" s="52"/>
+      <c r="D91" s="53"/>
+      <c r="E91" s="54"/>
+      <c r="F91" s="54"/>
+      <c r="G91" s="54"/>
+      <c r="H91" s="54"/>
+      <c r="I91" s="54"/>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B92" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="C92" s="52"/>
+      <c r="D92" s="53"/>
+      <c r="E92" s="54"/>
+      <c r="F92" s="54"/>
+      <c r="G92" s="54"/>
+      <c r="H92" s="54"/>
+      <c r="I92" s="54"/>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B93" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="C93" s="52"/>
+      <c r="D93" s="53"/>
+      <c r="E93" s="54"/>
+      <c r="F93" s="54"/>
+      <c r="G93" s="54"/>
+      <c r="H93" s="54"/>
+      <c r="I93" s="54"/>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B94" s="23"/>
+      <c r="C94" s="24"/>
+      <c r="D94" s="24"/>
+      <c r="E94" s="24"/>
+      <c r="F94" s="24"/>
+      <c r="G94" s="24"/>
+      <c r="H94" s="24"/>
+      <c r="I94" s="25"/>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B95" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="C95" s="56"/>
+      <c r="D95" s="56"/>
+      <c r="E95" s="56"/>
+      <c r="F95" s="56"/>
+      <c r="G95" s="56"/>
+      <c r="H95" s="56"/>
+      <c r="I95" s="57"/>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B96" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C96" s="59"/>
+      <c r="D96" s="60"/>
+      <c r="E96" s="61"/>
+      <c r="F96" s="61"/>
+      <c r="G96" s="61"/>
+      <c r="H96" s="61"/>
+      <c r="I96" s="61"/>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B97" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="C97" s="59"/>
+      <c r="D97" s="60"/>
+      <c r="E97" s="61"/>
+      <c r="F97" s="61"/>
+      <c r="G97" s="61"/>
+      <c r="H97" s="61"/>
+      <c r="I97" s="61"/>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B98" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="C98" s="59"/>
+      <c r="D98" s="60"/>
+      <c r="E98" s="61"/>
+      <c r="F98" s="61"/>
+      <c r="G98" s="61"/>
+      <c r="H98" s="61"/>
+      <c r="I98" s="61"/>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B99" s="23"/>
+      <c r="C99" s="24"/>
+      <c r="D99" s="24"/>
+      <c r="E99" s="24"/>
+      <c r="F99" s="24"/>
+      <c r="G99" s="24"/>
+      <c r="H99" s="24"/>
+      <c r="I99" s="25"/>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B100" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C100" s="63"/>
+      <c r="D100" s="63"/>
+      <c r="E100" s="63"/>
+      <c r="F100" s="63"/>
+      <c r="G100" s="63"/>
+      <c r="H100" s="63"/>
+      <c r="I100" s="64"/>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B101" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="C101" s="66"/>
+      <c r="D101" s="67"/>
+      <c r="E101" s="68"/>
+      <c r="F101" s="68"/>
+      <c r="G101" s="68"/>
+      <c r="H101" s="68"/>
+      <c r="I101" s="68"/>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="C102" s="66"/>
+      <c r="D102" s="67"/>
+      <c r="E102" s="68"/>
+      <c r="F102" s="68"/>
+      <c r="G102" s="68"/>
+      <c r="H102" s="68"/>
+      <c r="I102" s="68"/>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B103" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="C103" s="66"/>
+      <c r="D103" s="67"/>
+      <c r="E103" s="68"/>
+      <c r="F103" s="68"/>
+      <c r="G103" s="68"/>
+      <c r="H103" s="68"/>
+      <c r="I103" s="68"/>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B104" s="23"/>
+      <c r="C104" s="24"/>
+      <c r="D104" s="24"/>
+      <c r="E104" s="24"/>
+      <c r="F104" s="24"/>
+      <c r="G104" s="24"/>
+      <c r="H104" s="24"/>
+      <c r="I104" s="25"/>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B105" s="69" t="s">
+        <v>64</v>
+      </c>
+      <c r="C105" s="70"/>
+      <c r="D105" s="70"/>
+      <c r="E105" s="70"/>
+      <c r="F105" s="70"/>
+      <c r="G105" s="70"/>
+      <c r="H105" s="70"/>
+      <c r="I105" s="71"/>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B106" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="C106" s="73"/>
+      <c r="D106" s="74"/>
+      <c r="E106" s="75"/>
+      <c r="F106" s="75"/>
+      <c r="G106" s="75"/>
+      <c r="H106" s="75"/>
+      <c r="I106" s="75"/>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B107" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="C107" s="73"/>
+      <c r="D107" s="74"/>
+      <c r="E107" s="75"/>
+      <c r="F107" s="75"/>
+      <c r="G107" s="75"/>
+      <c r="H107" s="75"/>
+      <c r="I107" s="75"/>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B108" s="72" t="s">
+        <v>48</v>
+      </c>
+      <c r="C108" s="73"/>
+      <c r="D108" s="74"/>
+      <c r="E108" s="75"/>
+      <c r="F108" s="75"/>
+      <c r="G108" s="75"/>
+      <c r="H108" s="75"/>
+      <c r="I108" s="75"/>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B109" s="23"/>
+      <c r="C109" s="24"/>
+      <c r="D109" s="24"/>
+      <c r="E109" s="24"/>
+      <c r="F109" s="24"/>
+      <c r="G109" s="24"/>
+      <c r="H109" s="24"/>
+      <c r="I109" s="25"/>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B110" s="69" t="s">
+        <v>65</v>
+      </c>
+      <c r="C110" s="70"/>
+      <c r="D110" s="70"/>
+      <c r="E110" s="70"/>
+      <c r="F110" s="70"/>
+      <c r="G110" s="70"/>
+      <c r="H110" s="70"/>
+      <c r="I110" s="71"/>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B111" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="C111" s="73"/>
+      <c r="D111" s="74"/>
+      <c r="E111" s="75"/>
+      <c r="F111" s="75"/>
+      <c r="G111" s="75"/>
+      <c r="H111" s="75"/>
+      <c r="I111" s="75"/>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B112" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="C112" s="73"/>
+      <c r="D112" s="74"/>
+      <c r="E112" s="75"/>
+      <c r="F112" s="75"/>
+      <c r="G112" s="75"/>
+      <c r="H112" s="75"/>
+      <c r="I112" s="75"/>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B113" s="72" t="s">
+        <v>48</v>
+      </c>
+      <c r="C113" s="73"/>
+      <c r="D113" s="74"/>
+      <c r="E113" s="75"/>
+      <c r="F113" s="75"/>
+      <c r="G113" s="75"/>
+      <c r="H113" s="75"/>
+      <c r="I113" s="75"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
+  <mergeCells count="92">
+    <mergeCell ref="B113:D113"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="B108:D108"/>
+    <mergeCell ref="B109:I109"/>
+    <mergeCell ref="B110:I110"/>
+    <mergeCell ref="B111:D111"/>
+    <mergeCell ref="B112:D112"/>
+    <mergeCell ref="B103:D103"/>
+    <mergeCell ref="B104:I104"/>
+    <mergeCell ref="B105:I105"/>
+    <mergeCell ref="B106:D106"/>
+    <mergeCell ref="B107:D107"/>
+    <mergeCell ref="B98:D98"/>
+    <mergeCell ref="B99:I99"/>
+    <mergeCell ref="B100:I100"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B102:D102"/>
+    <mergeCell ref="B93:D93"/>
+    <mergeCell ref="B94:I94"/>
+    <mergeCell ref="B95:I95"/>
+    <mergeCell ref="B96:D96"/>
+    <mergeCell ref="B97:D97"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="B89:I89"/>
+    <mergeCell ref="B90:I90"/>
+    <mergeCell ref="B91:D91"/>
+    <mergeCell ref="B92:D92"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="B86:I86"/>
+    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="B82:I82"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B28:F28"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:K4"/>
-    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B32:F32"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B7:F7"/>
@@ -2625,15 +3755,22 @@
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B12:K12"/>
     <mergeCell ref="B13:K13"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>